<commit_message>
Added new labels to Dashboard
</commit_message>
<xml_diff>
--- a/inputs/Quantum Metric.xlsx
+++ b/inputs/Quantum Metric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julialiu/Files/Work/Greycroft/greycroft/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D031CE7F-DFB5-1947-88C0-0E38AA722168}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A9C4FA-42E8-1140-A303-9372A68B6EB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21940" windowHeight="16420" tabRatio="782" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21940" windowHeight="16420" tabRatio="782" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IS (2017)" sheetId="153" r:id="rId1"/>
@@ -1617,7 +1617,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="398">
   <si>
     <t>x</t>
   </si>
@@ -2803,6 +2803,15 @@
   <si>
     <t>Labels</t>
   </si>
+  <si>
+    <t>Net cash provided by operating activities</t>
+  </si>
+  <si>
+    <t>Net cash provided by investing activities</t>
+  </si>
+  <si>
+    <t>Net cash provided by financing activities</t>
+  </si>
 </sst>
 </file>
 
@@ -3176,7 +3185,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="39"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="39" applyAlignment="1"/>
@@ -3251,6 +3260,7 @@
     <xf numFmtId="44" fontId="28" fillId="0" borderId="2" xfId="45" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="45" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="6" xfId="45" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="Comma" xfId="17" builtinId="3"/>
@@ -10746,7 +10756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A18DE17-CF2F-7D47-ADC4-D9080974774D}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A20" sqref="A20"/>
       <selection pane="topRight" activeCell="A20" sqref="A20"/>
@@ -41811,12 +41821,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338C6F6A-986E-4D60-BC8B-720D86D1ADF1}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A20" sqref="A20"/>
       <selection pane="topRight" activeCell="A20" sqref="A20"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomRight" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -42153,6 +42163,9 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="48" t="s">
+        <v>395</v>
+      </c>
       <c r="B9" s="28" t="s">
         <v>385</v>
       </c>
@@ -42344,6 +42357,9 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="48" t="s">
+        <v>396</v>
+      </c>
       <c r="B14" s="28" t="s">
         <v>389</v>
       </c>
@@ -42490,6 +42506,9 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="48" t="s">
+        <v>397</v>
+      </c>
       <c r="B18" s="28" t="s">
         <v>392</v>
       </c>

</xml_diff>